<commit_message>
worked on highlevel testcases where it comes from xls
</commit_message>
<xml_diff>
--- a/Test_data.xlsx
+++ b/Test_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qamacbookpro/Desktop/latest_prospecta/latest_master_prospecta/test_automation_script/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qamacbookpro/bkp_07_08/test_automation_script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26BC8403-F0F2-7842-9A5C-02F4CA3B8CF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47C9667C-D1B1-C140-A67B-CBE203D9F4F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{00440C1E-4470-8B4B-8419-B8CD22275F29}"/>
   </bookViews>
@@ -417,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D3B4BEC-A60A-784B-99D1-7AB6D909C2A6}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -471,6 +471,11 @@
         <v>10</v>
       </c>
     </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>